<commit_message>
add some missed words
</commit_message>
<xml_diff>
--- a/utils/transliteration_data/_quran_freq_dv.xlsx
+++ b/utils/transliteration_data/_quran_freq_dv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Quran-Translation\utils\transliteration_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E511E5-C1A8-4617-8CC8-C4BDFBBA9306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{AFDE264A-5CB8-406B-B13B-9E3E28030CAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">arabic_freq!$A$1:$D$819</definedName>
+    <definedName name="ExternalData_1" localSheetId="1" hidden="1">arabic_freq!$A$1:$D$820</definedName>
     <definedName name="ExternalData_1" localSheetId="2" hidden="1">thaana_data!$A$1:$D$814</definedName>
     <definedName name="ExternalData_2" localSheetId="0" hidden="1">word_map!$A$1:$B$739</definedName>
   </definedNames>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5326" uniqueCount="1890">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5329" uniqueCount="1892">
   <si>
     <t>ar</t>
   </si>
@@ -5724,6 +5724,12 @@
   </si>
   <si>
     <t>ޙާކިމު</t>
+  </si>
+  <si>
+    <t>މުތަޝާބިހު</t>
+  </si>
+  <si>
+    <t>އަލްބައިތުލް މަޢުމޫރު</t>
   </si>
 </sst>
 </file>
@@ -6367,8 +6373,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="arabic_freq" displayName="arabic_freq" ref="A1:F819" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:F819" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="arabic_freq" displayName="arabic_freq" ref="A1:F820" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:F820" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="ar" queryTableFieldId="1" dataDxfId="3"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="dv" queryTableFieldId="4" dataDxfId="2"/>
@@ -12638,10 +12644,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F819"/>
+  <dimension ref="A1:F820"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A394" workbookViewId="0">
-      <selection activeCell="F410" sqref="F410"/>
+    <sheetView tabSelected="1" topLeftCell="A748" workbookViewId="0">
+      <selection activeCell="H765" sqref="H765"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -21047,8 +21053,13 @@
       <c r="A760" s="1" t="s">
         <v>1042</v>
       </c>
-      <c r="B760" s="2"/>
+      <c r="B760" s="2" t="s">
+        <v>1891</v>
+      </c>
       <c r="C760">
+        <v>1</v>
+      </c>
+      <c r="D760">
         <v>1</v>
       </c>
     </row>
@@ -21705,6 +21716,14 @@
       </c>
       <c r="C819">
         <v>1</v>
+      </c>
+    </row>
+    <row r="820" spans="1:3">
+      <c r="A820" s="1" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B820" s="2" t="s">
+        <v>1890</v>
       </c>
     </row>
   </sheetData>
@@ -21721,8 +21740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D814"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A442" sqref="A442"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>